<commit_message>
fix export, get all điểm
</commit_message>
<xml_diff>
--- a/kma_mm/kma_be/src/exports/excel/danh_gia_diem_qua_trinh.xlsx
+++ b/kma_mm/kma_be/src/exports/excel/danh_gia_diem_qua_trinh.xlsx
@@ -6,12 +6,15 @@
   <sheets>
     <sheet sheetId="1" name="SinhVien" state="visible" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'SinhVien'!$13:$14</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="81">
   <si>
     <t>HỌC VIỆN KỸ THUẬT MẬT MÃ</t>
   </si>
@@ -28,28 +31,112 @@
     <t>KẾT QUẢ ĐÁNH GIÁ ĐIỂM QUÁ TRÌNH</t>
   </si>
   <si>
-    <t>HỌC KỲ 1 NĂM HỌC 2024 - 2025</t>
-  </si>
-  <si>
-    <t>Học phần:</t>
-  </si>
-  <si>
-    <t>Số TC:</t>
-  </si>
-  <si>
-    <t>Mã học phần:</t>
-  </si>
-  <si>
-    <t>Lớp học phần:</t>
-  </si>
-  <si>
-    <t>Khoá:</t>
-  </si>
-  <si>
-    <t>Giảng viên giảng dạy:</t>
-  </si>
-  <si>
-    <t>Tổng số SV:</t>
+    <t>HỌC KỲ 1 NĂM HỌC 2021 - 2022</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Học phần: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Tin học đại cương</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Số TC: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Mã học phần: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>HMCTHT1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Lớp học phần: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>HH3101</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Khoá: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>HH31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Giảng viên giảng dạy: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="13"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Nguyễn Đức Hiếu</t>
+    </r>
+  </si>
+  <si>
+    <t>Tổng số SV: 16</t>
   </si>
   <si>
     <t>Số SV dự thi: ... Vắng ... Có lý do ... Không lý do ...</t>
@@ -91,37 +178,160 @@
     <t>Bằng chữ</t>
   </si>
   <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>CTL30101</t>
-  </si>
-  <si>
-    <t>Nguyễn A</t>
-  </si>
-  <si>
-    <t>CTL301</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>HH310101</t>
+  </si>
+  <si>
+    <t>Trần Xuân An</t>
+  </si>
+  <si>
+    <t>HH3101</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>CTL30102</t>
-  </si>
-  <si>
-    <t>Nguyễn B</t>
-  </si>
-  <si>
-    <t>Hà Nội, ngày 30 tháng 12 năm 2024</t>
+    <t>2</t>
+  </si>
+  <si>
+    <t>HH310102</t>
+  </si>
+  <si>
+    <t>Tưởng Cao Bằng</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>HH310103</t>
+  </si>
+  <si>
+    <t>Noy Boutdavongsy</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>HH310104</t>
+  </si>
+  <si>
+    <t>Nguyễn Đặng Dương</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>HH310105</t>
+  </si>
+  <si>
+    <t>Hoàng Viết Đức</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>HH310106</t>
+  </si>
+  <si>
+    <t>Nguyễn Ngọc Hải</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>HH310107</t>
+  </si>
+  <si>
+    <t>Lê Minh Hiếu</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>HH310108</t>
+  </si>
+  <si>
+    <t>Nguyễn Nam Khánh</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>HH310109</t>
+  </si>
+  <si>
+    <t>Khamphouthay Khuangboun</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>HH310110</t>
+  </si>
+  <si>
+    <t>Bùi Nguyễn Thành Lộc</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>HH310111</t>
+  </si>
+  <si>
+    <t>Đỗ Hoài Nam</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>HH310112</t>
+  </si>
+  <si>
+    <t>Bounsack Philaxay</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>HH310113</t>
+  </si>
+  <si>
+    <t>Nguyễn Trọng Quyết</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>HH310114</t>
+  </si>
+  <si>
+    <t>Oudomphone Thavone</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>HH310115</t>
+  </si>
+  <si>
+    <t>Lê Phi Trọng</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>HH310116</t>
+  </si>
+  <si>
+    <t>Phaivone Vilaphanh</t>
+  </si>
+  <si>
+    <t>Hà Nội, ngày ... tháng ... năm 20...</t>
   </si>
   <si>
     <t>GIẢNG VIÊN CHẤM THI</t>
-  </si>
-  <si>
-    <t>CHỦ NHIỆM BỘ MÔN</t>
   </si>
   <si>
     <t>GIÁO VỤ KHOA</t>
@@ -634,7 +844,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N36"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
@@ -885,7 +1095,7 @@
         <v>29</v>
       </c>
       <c r="I15" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J15" s="8">
         <v>10</v>
@@ -902,107 +1112,579 @@
       <c r="N15" s="8"/>
     </row>
     <row r="16" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="9">
+      <c r="I16" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="J16" s="8">
+        <v>8</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" s="8"/>
+    </row>
+    <row r="17" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="8">
+        <v>10</v>
+      </c>
+      <c r="J17" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" s="8"/>
+    </row>
+    <row r="18" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="8">
+        <v>8</v>
+      </c>
+      <c r="J18" s="8">
+        <v>9</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="J19" s="8">
+        <v>9.5</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="8">
+        <v>9</v>
+      </c>
+      <c r="J20" s="8">
+        <v>7</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" s="8"/>
+    </row>
+    <row r="21" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="8">
+        <v>9.5</v>
+      </c>
+      <c r="J21" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="8">
+        <v>7</v>
+      </c>
+      <c r="J22" s="8">
+        <v>8</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N22" s="8"/>
+    </row>
+    <row r="23" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="J23" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="8">
+        <v>8</v>
+      </c>
+      <c r="J24" s="8">
         <v>5</v>
       </c>
-      <c r="J16" s="9">
+      <c r="K24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" s="8"/>
+    </row>
+    <row r="25" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="8">
+        <v>8.5</v>
+      </c>
+      <c r="J25" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" s="8"/>
+    </row>
+    <row r="26" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="8">
         <v>5</v>
       </c>
-      <c r="K16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="J26" s="8">
+        <v>6</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="J27" s="8">
+        <v>7</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I28" s="8">
+        <v>6</v>
+      </c>
+      <c r="J28" s="8">
+        <v>7.5</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="8">
+        <v>7</v>
+      </c>
+      <c r="J29" s="8">
+        <v>4</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="J30" s="9">
+        <v>3</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" s="9"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="56">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:N1"/>
     <mergeCell ref="A2:C2"/>
@@ -1024,17 +1706,44 @@
     <mergeCell ref="M15:N15"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="M16:N16"/>
-    <mergeCell ref="J20:N20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:N21"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:N22"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="M25:N25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="C28:G28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="L36:N36"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="0"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.4" right="0.4" top="0.2" bottom="0.2" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
thêm quyền duyệt, sửa excel gk/ck không đúng thứ tự, xuất thông tin sv
</commit_message>
<xml_diff>
--- a/kma_mm/kma_be/src/exports/excel/danh_gia_diem_qua_trinh.xlsx
+++ b/kma_mm/kma_be/src/exports/excel/danh_gia_diem_qua_trinh.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>HỌC VIỆN KỸ THUẬT MẬT MÃ</t>
   </si>
@@ -31,7 +31,7 @@
     <t>KẾT QUẢ ĐÁNH GIÁ ĐIỂM QUÁ TRÌNH</t>
   </si>
   <si>
-    <t>HỌC KỲ 1 NĂM HỌC 2019 - 2020</t>
+    <t>HỌC KỲ 1 NĂM HỌC 2021 - 2022</t>
   </si>
   <si>
     <r>
@@ -47,7 +47,7 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>Lập trình driver</t>
+      <t>test1</t>
     </r>
   </si>
   <si>
@@ -81,7 +81,7 @@
         <sz val="10"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>LTD</t>
+      <t>test1</t>
     </r>
   </si>
   <si>
@@ -98,7 +98,7 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>ATL2201</t>
+      <t>test01</t>
     </r>
   </si>
   <si>
@@ -115,7 +115,7 @@
         <sz val="11"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t>ATL22</t>
+      <t>test</t>
     </r>
   </si>
   <si>
@@ -136,7 +136,7 @@
     </r>
   </si>
   <si>
-    <t>Tổng số SV: 4</t>
+    <t>Tổng số SV: 6</t>
   </si>
   <si>
     <t>Số SV dự thi: ... Vắng ... Có lý do ... Không lý do ...</t>
@@ -181,13 +181,13 @@
     <t>1</t>
   </si>
   <si>
-    <t>ATL220101</t>
-  </si>
-  <si>
-    <t>Nguyễn Tùng Dương</t>
-  </si>
-  <si>
-    <t>ATL2201</t>
+    <t>test0102</t>
+  </si>
+  <si>
+    <t>Lê Thị Bình</t>
+  </si>
+  <si>
+    <t>test01</t>
   </si>
   <si>
     <t/>
@@ -196,31 +196,46 @@
     <t>2</t>
   </si>
   <si>
-    <t>ATL220102</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Phú Thịnh</t>
+    <t>test0103</t>
+  </si>
+  <si>
+    <t>Cao Huy Cường</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>ATL200101</t>
-  </si>
-  <si>
-    <t>Nguyễn Huy Hoàng</t>
-  </si>
-  <si>
-    <t>ATL2001</t>
+    <t>test0104</t>
+  </si>
+  <si>
+    <t>Phạm Minh Dũng</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>ATL200102</t>
-  </si>
-  <si>
-    <t>Nguyễn Huy Phúc</t>
+    <t>test0101</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Hòa</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>test0105</t>
+  </si>
+  <si>
+    <t>Vũ Hưng</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>test0106</t>
+  </si>
+  <si>
+    <t>Nguyễn Quý Huy</t>
   </si>
   <si>
     <t>Hà Nội, ngày ... tháng ... năm 20...</t>
@@ -739,7 +754,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:O26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5.5" customWidth="1"/>
@@ -756,7 +771,7 @@
     <col min="13" max="14" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,18 +780,19 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -785,16 +801,17 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -990,10 +1007,10 @@
         <v>29</v>
       </c>
       <c r="I15" s="8">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J15" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>30</v>
@@ -1027,7 +1044,7 @@
         <v>8</v>
       </c>
       <c r="J16" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>30</v>
@@ -1055,13 +1072,13 @@
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I17" s="8">
         <v>7</v>
       </c>
       <c r="J17" s="8">
-        <v>8</v>
+        <v>6.5</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>30</v>
@@ -1075,107 +1092,175 @@
       <c r="N17" s="8"/>
     </row>
     <row r="18" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="8">
+        <v>7</v>
+      </c>
+      <c r="J18" s="8">
+        <v>8.2</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I18" s="9">
-        <v>9</v>
-      </c>
-      <c r="J18" s="9">
-        <v>9</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="C19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="11" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="8">
+        <v>6</v>
+      </c>
+      <c r="J19" s="8">
+        <v>7</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" s="8"/>
+    </row>
+    <row r="20" ht="16" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="11" t="s">
+      <c r="B20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
+      <c r="C20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="9">
+        <v>5</v>
+      </c>
+      <c r="J20" s="9">
+        <v>5</v>
+      </c>
+      <c r="K20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" s="9"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:N1"/>
+  <mergeCells count="36">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="H1:O1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="H2:O2"/>
     <mergeCell ref="A3:N3"/>
     <mergeCell ref="A4:N4"/>
     <mergeCell ref="A5:N5"/>
@@ -1197,13 +1282,17 @@
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="M18:N18"/>
-    <mergeCell ref="J22:N22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="L23:N23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="L24:N24"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="L26:N26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.4" right="0.4" top="0.2" bottom="0.2" header="0.3" footer="0.3"/>

</xml_diff>